<commit_message>
20.03.06 PM 20:24 Lot 속성 부여 로직 작성 중
Signed-off-by: shchoi <hoonse7758@naver.com>
</commit_message>
<xml_diff>
--- a/data/prod_yield.xlsx
+++ b/data/prod_yield.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
   <si>
     <t>GRADE_B</t>
   </si>
@@ -507,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -633,10 +633,10 @@
         <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
@@ -644,10 +644,10 @@
         <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
@@ -688,10 +688,10 @@
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
@@ -699,10 +699,10 @@
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
@@ -743,10 +743,10 @@
         <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
@@ -754,10 +754,10 @@
         <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
@@ -798,10 +798,10 @@
         <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C26">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
@@ -809,10 +809,10 @@
         <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
@@ -853,10 +853,10 @@
         <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C31">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
@@ -864,10 +864,10 @@
         <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
@@ -908,10 +908,10 @@
         <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C36">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
@@ -919,10 +919,10 @@
         <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
@@ -963,10 +963,10 @@
         <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C41">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
@@ -974,10 +974,10 @@
         <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
@@ -1018,10 +1018,10 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C46">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.4">
@@ -1029,10 +1029,10 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.4">
@@ -1065,446 +1065,6 @@
         <v>47</v>
       </c>
       <c r="C50">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A54" t="s">
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>11</v>
-      </c>
-      <c r="C54">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
-        <v>53</v>
-      </c>
-      <c r="B56" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
-        <v>53</v>
-      </c>
-      <c r="B58" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
-        <v>53</v>
-      </c>
-      <c r="B59" t="s">
-        <v>16</v>
-      </c>
-      <c r="C59">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A60" t="s">
-        <v>53</v>
-      </c>
-      <c r="B60" t="s">
-        <v>17</v>
-      </c>
-      <c r="C60">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
-        <v>53</v>
-      </c>
-      <c r="B61" t="s">
-        <v>18</v>
-      </c>
-      <c r="C61">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
-        <v>53</v>
-      </c>
-      <c r="B62" t="s">
-        <v>19</v>
-      </c>
-      <c r="C62">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
-        <v>53</v>
-      </c>
-      <c r="B63" t="s">
-        <v>20</v>
-      </c>
-      <c r="C63">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
-        <v>53</v>
-      </c>
-      <c r="B64" t="s">
-        <v>21</v>
-      </c>
-      <c r="C64">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
-        <v>53</v>
-      </c>
-      <c r="B65" t="s">
-        <v>22</v>
-      </c>
-      <c r="C65">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A66" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66" t="s">
-        <v>23</v>
-      </c>
-      <c r="C66">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A67" t="s">
-        <v>53</v>
-      </c>
-      <c r="B67" t="s">
-        <v>24</v>
-      </c>
-      <c r="C67">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A68" t="s">
-        <v>53</v>
-      </c>
-      <c r="B68" t="s">
-        <v>25</v>
-      </c>
-      <c r="C68">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A69" t="s">
-        <v>53</v>
-      </c>
-      <c r="B69" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A70" t="s">
-        <v>53</v>
-      </c>
-      <c r="B70" t="s">
-        <v>27</v>
-      </c>
-      <c r="C70">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A71" t="s">
-        <v>53</v>
-      </c>
-      <c r="B71" t="s">
-        <v>28</v>
-      </c>
-      <c r="C71">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A72" t="s">
-        <v>53</v>
-      </c>
-      <c r="B72" t="s">
-        <v>29</v>
-      </c>
-      <c r="C72">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A73" t="s">
-        <v>53</v>
-      </c>
-      <c r="B73" t="s">
-        <v>30</v>
-      </c>
-      <c r="C73">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A74" t="s">
-        <v>53</v>
-      </c>
-      <c r="B74" t="s">
-        <v>31</v>
-      </c>
-      <c r="C74">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A75" t="s">
-        <v>53</v>
-      </c>
-      <c r="B75" t="s">
-        <v>32</v>
-      </c>
-      <c r="C75">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A76" t="s">
-        <v>53</v>
-      </c>
-      <c r="B76" t="s">
-        <v>33</v>
-      </c>
-      <c r="C76">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A77" t="s">
-        <v>53</v>
-      </c>
-      <c r="B77" t="s">
-        <v>34</v>
-      </c>
-      <c r="C77">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A78" t="s">
-        <v>53</v>
-      </c>
-      <c r="B78" t="s">
-        <v>35</v>
-      </c>
-      <c r="C78">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A79" t="s">
-        <v>53</v>
-      </c>
-      <c r="B79" t="s">
-        <v>36</v>
-      </c>
-      <c r="C79">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A80" t="s">
-        <v>53</v>
-      </c>
-      <c r="B80" t="s">
-        <v>37</v>
-      </c>
-      <c r="C80">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A81" t="s">
-        <v>53</v>
-      </c>
-      <c r="B81" t="s">
-        <v>38</v>
-      </c>
-      <c r="C81">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A82" t="s">
-        <v>53</v>
-      </c>
-      <c r="B82" t="s">
-        <v>39</v>
-      </c>
-      <c r="C82">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A83" t="s">
-        <v>53</v>
-      </c>
-      <c r="B83" t="s">
-        <v>40</v>
-      </c>
-      <c r="C83">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A84" t="s">
-        <v>53</v>
-      </c>
-      <c r="B84" t="s">
-        <v>41</v>
-      </c>
-      <c r="C84">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A85" t="s">
-        <v>53</v>
-      </c>
-      <c r="B85" t="s">
-        <v>42</v>
-      </c>
-      <c r="C85">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A86" t="s">
-        <v>53</v>
-      </c>
-      <c r="B86" t="s">
-        <v>43</v>
-      </c>
-      <c r="C86">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A87" t="s">
-        <v>53</v>
-      </c>
-      <c r="B87" t="s">
-        <v>44</v>
-      </c>
-      <c r="C87">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A88" t="s">
-        <v>53</v>
-      </c>
-      <c r="B88" t="s">
-        <v>45</v>
-      </c>
-      <c r="C88">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A89" t="s">
-        <v>53</v>
-      </c>
-      <c r="B89" t="s">
-        <v>46</v>
-      </c>
-      <c r="C89">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A90" t="s">
-        <v>53</v>
-      </c>
-      <c r="B90" t="s">
-        <v>47</v>
-      </c>
-      <c r="C90">
         <v>40</v>
       </c>
     </row>

</xml_diff>